<commit_message>
RSD: remove water heating data input for HVO boiler providing only space heating
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_NewTechs.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFF2CD8-6F24-4D0D-A00A-C3DD5D1BE7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1307D6-DD79-43FD-9081-58A0901E9B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
@@ -15213,6 +15213,17 @@
     <xf numFmtId="2" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="72" fillId="38" borderId="0" xfId="18" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="72" fillId="38" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="72" fillId="38" borderId="0" xfId="18"/>
+    <xf numFmtId="166" fontId="73" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="73" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -15258,15 +15269,6 @@
     <xf numFmtId="0" fontId="54" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -15274,6 +15276,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15285,17 +15296,26 @@
     <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -15306,19 +15326,10 @@
     <xf numFmtId="0" fontId="17" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="61" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15336,6 +15347,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -15351,23 +15368,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="72" fillId="38" borderId="0" xfId="18" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="72" fillId="38" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="72" fillId="38" borderId="0" xfId="18"/>
-    <xf numFmtId="166" fontId="73" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="73" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="20% - Colore 2" xfId="11" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -17080,14 +17080,14 @@
       <c r="F16" s="211"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="562" t="s">
+      <c r="A17" s="569" t="s">
         <v>434</v>
       </c>
-      <c r="B17" s="562"/>
-      <c r="C17" s="562"/>
-      <c r="D17" s="562"/>
-      <c r="E17" s="562"/>
-      <c r="F17" s="562"/>
+      <c r="B17" s="569"/>
+      <c r="C17" s="569"/>
+      <c r="D17" s="569"/>
+      <c r="E17" s="569"/>
+      <c r="F17" s="569"/>
       <c r="G17" s="213"/>
       <c r="H17" s="213"/>
       <c r="I17" s="214"/>
@@ -17125,13 +17125,13 @@
       <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="563" t="s">
+      <c r="B20" s="570" t="s">
         <v>436</v>
       </c>
-      <c r="C20" s="563"/>
-      <c r="D20" s="563"/>
-      <c r="E20" s="563"/>
-      <c r="F20" s="563"/>
+      <c r="C20" s="570"/>
+      <c r="D20" s="570"/>
+      <c r="E20" s="570"/>
+      <c r="F20" s="570"/>
       <c r="G20" s="218"/>
       <c r="H20" s="218"/>
       <c r="I20" s="219"/>
@@ -17145,13 +17145,13 @@
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="564" t="s">
+      <c r="B21" s="571" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="564"/>
-      <c r="D21" s="564"/>
-      <c r="E21" s="564"/>
-      <c r="F21" s="564"/>
+      <c r="C21" s="571"/>
+      <c r="D21" s="571"/>
+      <c r="E21" s="571"/>
+      <c r="F21" s="571"/>
       <c r="G21" s="218"/>
       <c r="H21" s="218"/>
       <c r="I21" s="219"/>
@@ -17165,13 +17165,13 @@
       <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="564" t="s">
+      <c r="B22" s="571" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="564"/>
-      <c r="D22" s="564"/>
-      <c r="E22" s="564"/>
-      <c r="F22" s="564"/>
+      <c r="C22" s="571"/>
+      <c r="D22" s="571"/>
+      <c r="E22" s="571"/>
+      <c r="F22" s="571"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -17200,22 +17200,22 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="565"/>
-      <c r="B25" s="565"/>
-      <c r="C25" s="565"/>
-      <c r="D25" s="565"/>
-      <c r="E25" s="565"/>
-      <c r="F25" s="565"/>
+      <c r="A25" s="572"/>
+      <c r="B25" s="572"/>
+      <c r="C25" s="572"/>
+      <c r="D25" s="572"/>
+      <c r="E25" s="572"/>
+      <c r="F25" s="572"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="561"/>
-      <c r="B26" s="561"/>
-      <c r="C26" s="561"/>
-      <c r="D26" s="561"/>
-      <c r="E26" s="561"/>
-      <c r="F26" s="561"/>
+      <c r="A26" s="568"/>
+      <c r="B26" s="568"/>
+      <c r="C26" s="568"/>
+      <c r="D26" s="568"/>
+      <c r="E26" s="568"/>
+      <c r="F26" s="568"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="211"/>
@@ -17391,23 +17391,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="602" t="s">
+      <c r="A1" s="611" t="s">
         <v>1062</v>
       </c>
-      <c r="B1" s="604" t="s">
+      <c r="B1" s="613" t="s">
         <v>1063</v>
       </c>
-      <c r="C1" s="605"/>
-      <c r="D1" s="605"/>
-      <c r="E1" s="605"/>
-      <c r="F1" s="606"/>
-      <c r="G1" s="604" t="s">
+      <c r="C1" s="614"/>
+      <c r="D1" s="614"/>
+      <c r="E1" s="614"/>
+      <c r="F1" s="615"/>
+      <c r="G1" s="613" t="s">
         <v>1064</v>
       </c>
-      <c r="H1" s="605"/>
-      <c r="I1" s="605"/>
-      <c r="J1" s="605"/>
-      <c r="K1" s="606"/>
+      <c r="H1" s="614"/>
+      <c r="I1" s="614"/>
+      <c r="J1" s="614"/>
+      <c r="K1" s="615"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -17417,7 +17417,7 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="603"/>
+      <c r="A2" s="612"/>
       <c r="B2" s="527" t="s">
         <v>686</v>
       </c>
@@ -17563,12 +17563,12 @@
       <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="601" t="s">
+      <c r="A7" s="608" t="s">
         <v>1065</v>
       </c>
-      <c r="B7" s="601"/>
-      <c r="C7" s="601"/>
-      <c r="D7" s="601"/>
+      <c r="B7" s="608"/>
+      <c r="C7" s="608"/>
+      <c r="D7" s="608"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -17854,12 +17854,12 @@
       <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="601" t="s">
+      <c r="A18" s="608" t="s">
         <v>1079</v>
       </c>
-      <c r="B18" s="601"/>
-      <c r="C18" s="601"/>
-      <c r="D18" s="601"/>
+      <c r="B18" s="608"/>
+      <c r="C18" s="608"/>
+      <c r="D18" s="608"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -18114,12 +18114,12 @@
       <c r="R27" s="5"/>
     </row>
     <row r="28" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="601" t="s">
+      <c r="A28" s="608" t="s">
         <v>1087</v>
       </c>
-      <c r="B28" s="601"/>
-      <c r="C28" s="601"/>
-      <c r="D28" s="601"/>
+      <c r="B28" s="608"/>
+      <c r="C28" s="608"/>
+      <c r="D28" s="608"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -18607,12 +18607,12 @@
       </c>
     </row>
     <row r="40" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="601" t="s">
+      <c r="A40" s="608" t="s">
         <v>1068</v>
       </c>
-      <c r="B40" s="601"/>
-      <c r="C40" s="601"/>
-      <c r="D40" s="601"/>
+      <c r="B40" s="608"/>
+      <c r="C40" s="608"/>
+      <c r="D40" s="608"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -18788,12 +18788,12 @@
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="601" t="s">
+      <c r="A45" s="608" t="s">
         <v>1096</v>
       </c>
-      <c r="B45" s="601"/>
-      <c r="C45" s="601"/>
-      <c r="D45" s="601"/>
+      <c r="B45" s="608"/>
+      <c r="C45" s="608"/>
+      <c r="D45" s="608"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -18910,11 +18910,11 @@
       <c r="Y48" t="s">
         <v>1113</v>
       </c>
-      <c r="Z48" s="607" t="s">
+      <c r="Z48" s="609" t="s">
         <v>1051</v>
       </c>
-      <c r="AA48" s="608"/>
-      <c r="AB48" s="608"/>
+      <c r="AA48" s="610"/>
+      <c r="AB48" s="610"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -19131,11 +19131,11 @@
       <c r="Y53" t="s">
         <v>1115</v>
       </c>
-      <c r="Z53" s="607" t="s">
+      <c r="Z53" s="609" t="s">
         <v>1050</v>
       </c>
-      <c r="AA53" s="608"/>
-      <c r="AB53" s="608"/>
+      <c r="AA53" s="610"/>
+      <c r="AB53" s="610"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -19342,11 +19342,11 @@
       <c r="Y59" t="s">
         <v>1116</v>
       </c>
-      <c r="Z59" s="607" t="s">
+      <c r="Z59" s="609" t="s">
         <v>1117</v>
       </c>
-      <c r="AA59" s="608"/>
-      <c r="AB59" s="608"/>
+      <c r="AA59" s="610"/>
+      <c r="AB59" s="610"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="547" t="str">
@@ -20244,17 +20244,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="71" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20289,16 +20289,16 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="566" t="s">
+      <c r="B2" s="573" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="567"/>
-      <c r="D2" s="567"/>
-      <c r="E2" s="568"/>
-      <c r="G2" s="566" t="s">
+      <c r="C2" s="574"/>
+      <c r="D2" s="574"/>
+      <c r="E2" s="575"/>
+      <c r="G2" s="573" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="568"/>
+      <c r="H2" s="575"/>
       <c r="I2" s="222"/>
       <c r="J2" s="222"/>
       <c r="K2" s="223"/>
@@ -20640,16 +20640,16 @@
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="569" t="s">
+      <c r="B20" s="576" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="570"/>
-      <c r="D20" s="570"/>
-      <c r="E20" s="571"/>
-      <c r="G20" s="566" t="s">
+      <c r="C20" s="577"/>
+      <c r="D20" s="577"/>
+      <c r="E20" s="578"/>
+      <c r="G20" s="573" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="568"/>
+      <c r="H20" s="575"/>
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="250" t="s">
@@ -20893,16 +20893,16 @@
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="566" t="s">
+      <c r="B38" s="573" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="567"/>
-      <c r="D38" s="567"/>
-      <c r="E38" s="568"/>
-      <c r="G38" s="572" t="s">
+      <c r="C38" s="574"/>
+      <c r="D38" s="574"/>
+      <c r="E38" s="575"/>
+      <c r="G38" s="579" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="573"/>
+      <c r="H38" s="580"/>
     </row>
     <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="271" t="s">
@@ -21071,13 +21071,13 @@
       <c r="M3" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="S3" s="574" t="s">
+      <c r="S3" s="581" t="s">
         <v>680</v>
       </c>
-      <c r="T3" s="574"/>
-      <c r="U3" s="574"/>
-      <c r="V3" s="574"/>
-      <c r="W3" s="574"/>
+      <c r="T3" s="581"/>
+      <c r="U3" s="581"/>
+      <c r="V3" s="581"/>
+      <c r="W3" s="581"/>
     </row>
     <row r="4" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="62" t="s">
@@ -21271,10 +21271,10 @@
         <v>5.6296955912135845E-4</v>
       </c>
       <c r="J9" s="103"/>
-      <c r="M9" s="575" t="s">
+      <c r="M9" s="582" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="575" t="s">
+      <c r="N9" s="582" t="s">
         <v>110</v>
       </c>
       <c r="S9" s="300" t="s">
@@ -28776,8 +28776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AR166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -28941,34 +28941,34 @@
       <c r="G4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H4" s="582" t="s">
+      <c r="H4" s="589" t="s">
         <v>719</v>
       </c>
-      <c r="I4" s="583"/>
-      <c r="J4" s="583"/>
-      <c r="K4" s="584"/>
-      <c r="L4" s="582" t="s">
+      <c r="I4" s="590"/>
+      <c r="J4" s="590"/>
+      <c r="K4" s="591"/>
+      <c r="L4" s="589" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="583"/>
-      <c r="N4" s="583"/>
-      <c r="O4" s="584"/>
-      <c r="P4" s="582" t="s">
+      <c r="M4" s="590"/>
+      <c r="N4" s="590"/>
+      <c r="O4" s="591"/>
+      <c r="P4" s="589" t="s">
         <v>320</v>
       </c>
-      <c r="Q4" s="583"/>
-      <c r="R4" s="583"/>
-      <c r="S4" s="584"/>
-      <c r="T4" s="582" t="s">
+      <c r="Q4" s="590"/>
+      <c r="R4" s="590"/>
+      <c r="S4" s="591"/>
+      <c r="T4" s="589" t="s">
         <v>321</v>
       </c>
-      <c r="U4" s="584"/>
-      <c r="V4" s="576" t="s">
+      <c r="U4" s="591"/>
+      <c r="V4" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="577"/>
-      <c r="X4" s="577"/>
-      <c r="Y4" s="578"/>
+      <c r="W4" s="593"/>
+      <c r="X4" s="593"/>
+      <c r="Y4" s="594"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -29067,34 +29067,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="579" t="s">
+      <c r="H6" s="583" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="580"/>
-      <c r="J6" s="580"/>
-      <c r="K6" s="581"/>
-      <c r="L6" s="580" t="s">
+      <c r="I6" s="584"/>
+      <c r="J6" s="584"/>
+      <c r="K6" s="585"/>
+      <c r="L6" s="584" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="580"/>
-      <c r="N6" s="580"/>
-      <c r="O6" s="581"/>
-      <c r="P6" s="579" t="s">
+      <c r="M6" s="584"/>
+      <c r="N6" s="584"/>
+      <c r="O6" s="585"/>
+      <c r="P6" s="583" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="580"/>
-      <c r="R6" s="580"/>
-      <c r="S6" s="581"/>
-      <c r="T6" s="579" t="s">
+      <c r="Q6" s="584"/>
+      <c r="R6" s="584"/>
+      <c r="S6" s="585"/>
+      <c r="T6" s="583" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="581"/>
-      <c r="V6" s="579" t="s">
+      <c r="U6" s="585"/>
+      <c r="V6" s="583" t="s">
         <v>967</v>
       </c>
-      <c r="W6" s="580"/>
-      <c r="X6" s="580"/>
-      <c r="Y6" s="581"/>
+      <c r="W6" s="584"/>
+      <c r="X6" s="584"/>
+      <c r="Y6" s="585"/>
       <c r="Z6" s="107" t="s">
         <v>979</v>
       </c>
@@ -31883,16 +31883,16 @@
       <c r="AI37" s="113">
         <v>5</v>
       </c>
-      <c r="AK37" s="609" t="s">
+      <c r="AK37" s="561" t="s">
         <v>1120</v>
       </c>
-      <c r="AL37" s="610"/>
-      <c r="AM37" s="610"/>
-      <c r="AN37" s="610"/>
-      <c r="AO37" s="610"/>
-      <c r="AP37" s="610"/>
-      <c r="AQ37" s="610"/>
-      <c r="AR37" s="611"/>
+      <c r="AL37" s="562"/>
+      <c r="AM37" s="562"/>
+      <c r="AN37" s="562"/>
+      <c r="AO37" s="562"/>
+      <c r="AP37" s="562"/>
+      <c r="AQ37" s="562"/>
+      <c r="AR37" s="563"/>
     </row>
     <row r="38" spans="3:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AK38" s="182" t="s">
@@ -31921,28 +31921,28 @@
       </c>
     </row>
     <row r="39" spans="3:44" ht="48.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AK39" s="612" t="s">
+      <c r="AK39" s="564" t="s">
         <v>1129</v>
       </c>
-      <c r="AL39" s="612" t="s">
+      <c r="AL39" s="564" t="s">
         <v>1130</v>
       </c>
-      <c r="AM39" s="612" t="s">
+      <c r="AM39" s="564" t="s">
         <v>1131</v>
       </c>
-      <c r="AN39" s="613" t="s">
+      <c r="AN39" s="565" t="s">
         <v>1124</v>
       </c>
-      <c r="AO39" s="613" t="s">
+      <c r="AO39" s="565" t="s">
         <v>1132</v>
       </c>
-      <c r="AP39" s="613" t="s">
+      <c r="AP39" s="565" t="s">
         <v>1133</v>
       </c>
-      <c r="AQ39" s="613" t="s">
+      <c r="AQ39" s="565" t="s">
         <v>1134</v>
       </c>
-      <c r="AR39" s="613" t="s">
+      <c r="AR39" s="565" t="s">
         <v>1135</v>
       </c>
     </row>
@@ -31950,27 +31950,27 @@
       <c r="H40" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AK40" s="614" t="str">
+      <c r="AK40" s="566" t="str">
         <f>AI40&amp;"NRG"</f>
         <v>NRG</v>
       </c>
-      <c r="AL40" s="614" t="s">
+      <c r="AL40" s="566" t="s">
         <v>1136</v>
       </c>
-      <c r="AM40" s="614" t="s">
+      <c r="AM40" s="566" t="s">
         <v>1137</v>
       </c>
-      <c r="AN40" s="615" t="s">
+      <c r="AN40" s="567" t="s">
         <v>16</v>
       </c>
-      <c r="AO40" s="614" t="s">
+      <c r="AO40" s="566" t="s">
         <v>914</v>
       </c>
-      <c r="AP40" s="614"/>
-      <c r="AQ40" s="614" t="s">
+      <c r="AP40" s="566"/>
+      <c r="AQ40" s="566" t="s">
         <v>914</v>
       </c>
-      <c r="AR40" s="614" t="s">
+      <c r="AR40" s="566" t="s">
         <v>914</v>
       </c>
     </row>
@@ -32091,34 +32091,34 @@
       <c r="G42" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H42" s="582" t="s">
+      <c r="H42" s="589" t="s">
         <v>318</v>
       </c>
-      <c r="I42" s="583"/>
-      <c r="J42" s="583"/>
-      <c r="K42" s="584"/>
-      <c r="L42" s="582" t="s">
+      <c r="I42" s="590"/>
+      <c r="J42" s="590"/>
+      <c r="K42" s="591"/>
+      <c r="L42" s="589" t="s">
         <v>319</v>
       </c>
-      <c r="M42" s="583"/>
-      <c r="N42" s="583"/>
-      <c r="O42" s="584"/>
-      <c r="P42" s="582" t="s">
+      <c r="M42" s="590"/>
+      <c r="N42" s="590"/>
+      <c r="O42" s="591"/>
+      <c r="P42" s="589" t="s">
         <v>320</v>
       </c>
-      <c r="Q42" s="583"/>
-      <c r="R42" s="583"/>
-      <c r="S42" s="584"/>
-      <c r="T42" s="582" t="s">
+      <c r="Q42" s="590"/>
+      <c r="R42" s="590"/>
+      <c r="S42" s="591"/>
+      <c r="T42" s="589" t="s">
         <v>321</v>
       </c>
-      <c r="U42" s="584"/>
-      <c r="V42" s="576" t="s">
+      <c r="U42" s="591"/>
+      <c r="V42" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="577"/>
-      <c r="X42" s="577"/>
-      <c r="Y42" s="578"/>
+      <c r="W42" s="593"/>
+      <c r="X42" s="593"/>
+      <c r="Y42" s="594"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -32217,34 +32217,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="579" t="s">
+      <c r="H44" s="583" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="580"/>
-      <c r="J44" s="580"/>
-      <c r="K44" s="581"/>
-      <c r="L44" s="580" t="s">
+      <c r="I44" s="584"/>
+      <c r="J44" s="584"/>
+      <c r="K44" s="585"/>
+      <c r="L44" s="584" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="580"/>
-      <c r="N44" s="580"/>
-      <c r="O44" s="581"/>
-      <c r="P44" s="579" t="s">
+      <c r="M44" s="584"/>
+      <c r="N44" s="584"/>
+      <c r="O44" s="585"/>
+      <c r="P44" s="583" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="580"/>
-      <c r="R44" s="580"/>
-      <c r="S44" s="581"/>
-      <c r="T44" s="585" t="s">
+      <c r="Q44" s="584"/>
+      <c r="R44" s="584"/>
+      <c r="S44" s="585"/>
+      <c r="T44" s="586" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="586"/>
-      <c r="V44" s="585" t="s">
+      <c r="U44" s="587"/>
+      <c r="V44" s="586" t="s">
         <v>967</v>
       </c>
-      <c r="W44" s="587"/>
-      <c r="X44" s="587"/>
-      <c r="Y44" s="586"/>
+      <c r="W44" s="588"/>
+      <c r="X44" s="588"/>
+      <c r="Y44" s="587"/>
       <c r="Z44" s="450" t="s">
         <v>979</v>
       </c>
@@ -33762,22 +33762,10 @@
       <c r="M59" s="77"/>
       <c r="N59" s="77"/>
       <c r="O59" s="89"/>
-      <c r="P59" s="86">
-        <f t="shared" si="44"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="Q59" s="75">
-        <f t="shared" si="44"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="R59" s="75">
-        <f t="shared" si="44"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="S59" s="104">
-        <f t="shared" si="44"/>
-        <v>0.57399999999999995</v>
-      </c>
+      <c r="P59" s="86"/>
+      <c r="Q59" s="75"/>
+      <c r="R59" s="75"/>
+      <c r="S59" s="104"/>
       <c r="T59" s="100">
         <v>20</v>
       </c>
@@ -36013,34 +36001,34 @@
       <c r="G90" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="H90" s="582" t="s">
+      <c r="H90" s="589" t="s">
         <v>318</v>
       </c>
-      <c r="I90" s="583"/>
-      <c r="J90" s="583"/>
-      <c r="K90" s="584"/>
-      <c r="L90" s="582" t="s">
+      <c r="I90" s="590"/>
+      <c r="J90" s="590"/>
+      <c r="K90" s="591"/>
+      <c r="L90" s="589" t="s">
         <v>319</v>
       </c>
-      <c r="M90" s="583"/>
-      <c r="N90" s="583"/>
-      <c r="O90" s="584"/>
-      <c r="P90" s="582" t="s">
+      <c r="M90" s="590"/>
+      <c r="N90" s="590"/>
+      <c r="O90" s="591"/>
+      <c r="P90" s="589" t="s">
         <v>320</v>
       </c>
-      <c r="Q90" s="583"/>
-      <c r="R90" s="583"/>
-      <c r="S90" s="584"/>
-      <c r="T90" s="582" t="s">
+      <c r="Q90" s="590"/>
+      <c r="R90" s="590"/>
+      <c r="S90" s="591"/>
+      <c r="T90" s="589" t="s">
         <v>321</v>
       </c>
-      <c r="U90" s="584"/>
-      <c r="V90" s="576" t="s">
+      <c r="U90" s="591"/>
+      <c r="V90" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="577"/>
-      <c r="X90" s="577"/>
-      <c r="Y90" s="578"/>
+      <c r="W90" s="593"/>
+      <c r="X90" s="593"/>
+      <c r="Y90" s="594"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -36139,34 +36127,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="579" t="s">
+      <c r="H92" s="583" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="580"/>
-      <c r="J92" s="580"/>
-      <c r="K92" s="581"/>
-      <c r="L92" s="580" t="s">
+      <c r="I92" s="584"/>
+      <c r="J92" s="584"/>
+      <c r="K92" s="585"/>
+      <c r="L92" s="584" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="580"/>
-      <c r="N92" s="580"/>
-      <c r="O92" s="581"/>
-      <c r="P92" s="579" t="s">
+      <c r="M92" s="584"/>
+      <c r="N92" s="584"/>
+      <c r="O92" s="585"/>
+      <c r="P92" s="583" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="580"/>
-      <c r="R92" s="580"/>
-      <c r="S92" s="581"/>
-      <c r="T92" s="585" t="s">
+      <c r="Q92" s="584"/>
+      <c r="R92" s="584"/>
+      <c r="S92" s="585"/>
+      <c r="T92" s="586" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="586"/>
-      <c r="V92" s="585" t="s">
+      <c r="U92" s="587"/>
+      <c r="V92" s="586" t="s">
         <v>967</v>
       </c>
-      <c r="W92" s="587"/>
-      <c r="X92" s="587"/>
-      <c r="Y92" s="586"/>
+      <c r="W92" s="588"/>
+      <c r="X92" s="588"/>
+      <c r="Y92" s="587"/>
       <c r="Z92" s="450" t="s">
         <v>979</v>
       </c>
@@ -37684,22 +37672,10 @@
       <c r="M107" s="77"/>
       <c r="N107" s="77"/>
       <c r="O107" s="89"/>
-      <c r="P107" s="86">
-        <f t="shared" si="83"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="Q107" s="75">
-        <f t="shared" si="84"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="R107" s="75">
-        <f t="shared" si="85"/>
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="S107" s="104">
-        <f t="shared" si="86"/>
-        <v>0.57399999999999995</v>
-      </c>
+      <c r="P107" s="86"/>
+      <c r="Q107" s="75"/>
+      <c r="R107" s="75"/>
+      <c r="S107" s="104"/>
       <c r="T107" s="100">
         <v>20</v>
       </c>
@@ -40097,26 +40073,6 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -40127,6 +40083,26 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -40271,12 +40247,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="576" t="s">
+      <c r="L5" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="577"/>
-      <c r="N5" s="577"/>
-      <c r="O5" s="578"/>
+      <c r="M5" s="593"/>
+      <c r="N5" s="593"/>
+      <c r="O5" s="594"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -40307,12 +40283,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="585" t="s">
+      <c r="L6" s="586" t="s">
         <v>967</v>
       </c>
-      <c r="M6" s="587"/>
-      <c r="N6" s="587"/>
-      <c r="O6" s="586"/>
+      <c r="M6" s="588"/>
+      <c r="N6" s="588"/>
+      <c r="O6" s="587"/>
       <c r="P6" s="450" t="s">
         <v>979</v>
       </c>
@@ -40938,10 +40914,10 @@
       <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="588" t="s">
+      <c r="R18" s="595" t="s">
         <v>662</v>
       </c>
-      <c r="S18" s="588"/>
+      <c r="S18" s="595"/>
       <c r="U18" s="5" t="s">
         <v>860</v>
       </c>
@@ -40974,8 +40950,8 @@
       <c r="J19" s="195" t="s">
         <v>301</v>
       </c>
-      <c r="R19" s="588"/>
-      <c r="S19" s="588"/>
+      <c r="R19" s="595"/>
+      <c r="S19" s="595"/>
       <c r="V19" s="5" t="s">
         <v>1021</v>
       </c>
@@ -41001,8 +40977,8 @@
       <c r="J20" s="170" t="s">
         <v>1026</v>
       </c>
-      <c r="R20" s="588"/>
-      <c r="S20" s="588"/>
+      <c r="R20" s="595"/>
+      <c r="S20" s="595"/>
       <c r="V20" s="5" t="s">
         <v>1022</v>
       </c>
@@ -41029,8 +41005,8 @@
       <c r="J21" s="170" t="s">
         <v>1026</v>
       </c>
-      <c r="R21" s="588"/>
-      <c r="S21" s="588"/>
+      <c r="R21" s="595"/>
+      <c r="S21" s="595"/>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C22" s="168" t="s">
@@ -41054,8 +41030,8 @@
       <c r="J22" s="170" t="s">
         <v>1026</v>
       </c>
-      <c r="R22" s="588"/>
-      <c r="S22" s="588"/>
+      <c r="R22" s="595"/>
+      <c r="S22" s="595"/>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.2">
       <c r="C23" s="168" t="s">
@@ -41230,23 +41206,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="576" t="s">
+      <c r="L33" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="577"/>
-      <c r="N33" s="577"/>
-      <c r="O33" s="578"/>
+      <c r="M33" s="593"/>
+      <c r="N33" s="593"/>
+      <c r="O33" s="594"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="585" t="s">
+      <c r="L34" s="586" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="587"/>
-      <c r="N34" s="587"/>
-      <c r="O34" s="586"/>
+      <c r="M34" s="588"/>
+      <c r="N34" s="588"/>
+      <c r="O34" s="587"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -41588,16 +41564,16 @@
       <c r="G4" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="H4" s="582" t="s">
+      <c r="H4" s="589" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="583"/>
-      <c r="J4" s="584"/>
-      <c r="K4" s="576" t="s">
+      <c r="I4" s="590"/>
+      <c r="J4" s="591"/>
+      <c r="K4" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="577"/>
-      <c r="M4" s="578"/>
+      <c r="L4" s="593"/>
+      <c r="M4" s="594"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -41623,16 +41599,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="589" t="s">
+      <c r="H5" s="599" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="590"/>
-      <c r="J5" s="591"/>
-      <c r="K5" s="589" t="s">
+      <c r="I5" s="600"/>
+      <c r="J5" s="601"/>
+      <c r="K5" s="599" t="s">
         <v>756</v>
       </c>
-      <c r="L5" s="590"/>
-      <c r="M5" s="591"/>
+      <c r="L5" s="600"/>
+      <c r="M5" s="601"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -41649,23 +41625,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="592" t="s">
+      <c r="AB5" s="596" t="s">
         <v>1011</v>
       </c>
-      <c r="AC5" s="592"/>
+      <c r="AC5" s="596"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="593" t="s">
+      <c r="AE5" s="597" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="593"/>
-      <c r="AG5" s="593" t="s">
+      <c r="AF5" s="597"/>
+      <c r="AG5" s="597" t="s">
         <v>1012</v>
       </c>
-      <c r="AH5" s="593"/>
-      <c r="AI5" s="594" t="s">
+      <c r="AH5" s="597"/>
+      <c r="AI5" s="598" t="s">
         <v>1013</v>
       </c>
-      <c r="AJ5" s="594"/>
+      <c r="AJ5" s="598"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -42403,12 +42379,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="576" t="s">
+      <c r="L27" s="592" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="577"/>
-      <c r="N27" s="577"/>
-      <c r="O27" s="578"/>
+      <c r="M27" s="593"/>
+      <c r="N27" s="593"/>
+      <c r="O27" s="594"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -42416,12 +42392,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="579" t="s">
+      <c r="L28" s="583" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="580"/>
-      <c r="N28" s="580"/>
-      <c r="O28" s="581"/>
+      <c r="M28" s="584"/>
+      <c r="N28" s="584"/>
+      <c r="O28" s="585"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -43811,16 +43787,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
     <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -52850,128 +52826,128 @@
       <c r="C4" s="356" t="s">
         <v>765</v>
       </c>
-      <c r="D4" s="595" t="s">
+      <c r="D4" s="603" t="s">
         <v>766</v>
       </c>
-      <c r="E4" s="596"/>
-      <c r="F4" s="596"/>
-      <c r="G4" s="596"/>
-      <c r="H4" s="597"/>
-      <c r="I4" s="596" t="s">
+      <c r="E4" s="602"/>
+      <c r="F4" s="602"/>
+      <c r="G4" s="602"/>
+      <c r="H4" s="604"/>
+      <c r="I4" s="602" t="s">
         <v>767</v>
       </c>
-      <c r="J4" s="596"/>
-      <c r="K4" s="596"/>
-      <c r="L4" s="596"/>
-      <c r="M4" s="597"/>
-      <c r="N4" s="596" t="s">
+      <c r="J4" s="602"/>
+      <c r="K4" s="602"/>
+      <c r="L4" s="602"/>
+      <c r="M4" s="604"/>
+      <c r="N4" s="602" t="s">
         <v>768</v>
       </c>
-      <c r="O4" s="596"/>
-      <c r="P4" s="596"/>
-      <c r="Q4" s="596"/>
-      <c r="R4" s="597"/>
-      <c r="S4" s="596" t="s">
+      <c r="O4" s="602"/>
+      <c r="P4" s="602"/>
+      <c r="Q4" s="602"/>
+      <c r="R4" s="604"/>
+      <c r="S4" s="602" t="s">
         <v>769</v>
       </c>
-      <c r="T4" s="596"/>
-      <c r="U4" s="596"/>
-      <c r="V4" s="596"/>
-      <c r="W4" s="597"/>
-      <c r="X4" s="596" t="s">
+      <c r="T4" s="602"/>
+      <c r="U4" s="602"/>
+      <c r="V4" s="602"/>
+      <c r="W4" s="604"/>
+      <c r="X4" s="602" t="s">
         <v>770</v>
       </c>
-      <c r="Y4" s="596"/>
-      <c r="Z4" s="596"/>
-      <c r="AA4" s="596"/>
-      <c r="AB4" s="597"/>
-      <c r="AC4" s="596" t="s">
+      <c r="Y4" s="602"/>
+      <c r="Z4" s="602"/>
+      <c r="AA4" s="602"/>
+      <c r="AB4" s="604"/>
+      <c r="AC4" s="602" t="s">
         <v>771</v>
       </c>
-      <c r="AD4" s="596"/>
-      <c r="AE4" s="596"/>
-      <c r="AF4" s="596"/>
-      <c r="AG4" s="597"/>
-      <c r="AH4" s="596" t="s">
+      <c r="AD4" s="602"/>
+      <c r="AE4" s="602"/>
+      <c r="AF4" s="602"/>
+      <c r="AG4" s="604"/>
+      <c r="AH4" s="602" t="s">
         <v>772</v>
       </c>
-      <c r="AI4" s="596"/>
-      <c r="AJ4" s="596"/>
-      <c r="AK4" s="596"/>
-      <c r="AL4" s="597"/>
-      <c r="AM4" s="596" t="s">
+      <c r="AI4" s="602"/>
+      <c r="AJ4" s="602"/>
+      <c r="AK4" s="602"/>
+      <c r="AL4" s="604"/>
+      <c r="AM4" s="602" t="s">
         <v>773</v>
       </c>
-      <c r="AN4" s="596"/>
-      <c r="AO4" s="596"/>
-      <c r="AP4" s="596"/>
-      <c r="AQ4" s="597"/>
-      <c r="AR4" s="596" t="s">
+      <c r="AN4" s="602"/>
+      <c r="AO4" s="602"/>
+      <c r="AP4" s="602"/>
+      <c r="AQ4" s="604"/>
+      <c r="AR4" s="602" t="s">
         <v>774</v>
       </c>
-      <c r="AS4" s="596"/>
-      <c r="AT4" s="596"/>
-      <c r="AU4" s="596"/>
-      <c r="AV4" s="597"/>
-      <c r="AW4" s="596" t="s">
+      <c r="AS4" s="602"/>
+      <c r="AT4" s="602"/>
+      <c r="AU4" s="602"/>
+      <c r="AV4" s="604"/>
+      <c r="AW4" s="602" t="s">
         <v>775</v>
       </c>
-      <c r="AX4" s="596"/>
-      <c r="AY4" s="596"/>
-      <c r="AZ4" s="596"/>
-      <c r="BA4" s="596"/>
-      <c r="BB4" s="595" t="s">
+      <c r="AX4" s="602"/>
+      <c r="AY4" s="602"/>
+      <c r="AZ4" s="602"/>
+      <c r="BA4" s="602"/>
+      <c r="BB4" s="603" t="s">
         <v>776</v>
       </c>
-      <c r="BC4" s="596"/>
-      <c r="BD4" s="596"/>
-      <c r="BE4" s="596"/>
-      <c r="BF4" s="597"/>
-      <c r="BG4" s="596" t="s">
+      <c r="BC4" s="602"/>
+      <c r="BD4" s="602"/>
+      <c r="BE4" s="602"/>
+      <c r="BF4" s="604"/>
+      <c r="BG4" s="602" t="s">
         <v>777</v>
       </c>
-      <c r="BH4" s="596"/>
-      <c r="BI4" s="596"/>
-      <c r="BJ4" s="596"/>
-      <c r="BK4" s="596"/>
-      <c r="BL4" s="595" t="s">
+      <c r="BH4" s="602"/>
+      <c r="BI4" s="602"/>
+      <c r="BJ4" s="602"/>
+      <c r="BK4" s="602"/>
+      <c r="BL4" s="603" t="s">
         <v>778</v>
       </c>
-      <c r="BM4" s="596"/>
-      <c r="BN4" s="596"/>
-      <c r="BO4" s="596"/>
-      <c r="BP4" s="596"/>
-      <c r="BQ4" s="595" t="s">
+      <c r="BM4" s="602"/>
+      <c r="BN4" s="602"/>
+      <c r="BO4" s="602"/>
+      <c r="BP4" s="602"/>
+      <c r="BQ4" s="603" t="s">
         <v>779</v>
       </c>
-      <c r="BR4" s="596"/>
-      <c r="BS4" s="596"/>
-      <c r="BT4" s="596"/>
-      <c r="BU4" s="597"/>
+      <c r="BR4" s="602"/>
+      <c r="BS4" s="602"/>
+      <c r="BT4" s="602"/>
+      <c r="BU4" s="604"/>
       <c r="BV4" s="357" t="s">
         <v>780</v>
       </c>
-      <c r="BW4" s="598" t="s">
+      <c r="BW4" s="605" t="s">
         <v>781</v>
       </c>
-      <c r="BX4" s="599"/>
-      <c r="BY4" s="599"/>
-      <c r="BZ4" s="599"/>
-      <c r="CA4" s="600"/>
-      <c r="CB4" s="598" t="s">
+      <c r="BX4" s="606"/>
+      <c r="BY4" s="606"/>
+      <c r="BZ4" s="606"/>
+      <c r="CA4" s="607"/>
+      <c r="CB4" s="605" t="s">
         <v>782</v>
       </c>
-      <c r="CC4" s="599"/>
-      <c r="CD4" s="599"/>
-      <c r="CE4" s="599"/>
-      <c r="CF4" s="600"/>
-      <c r="CG4" s="598" t="s">
+      <c r="CC4" s="606"/>
+      <c r="CD4" s="606"/>
+      <c r="CE4" s="606"/>
+      <c r="CF4" s="607"/>
+      <c r="CG4" s="605" t="s">
         <v>783</v>
       </c>
-      <c r="CH4" s="599"/>
-      <c r="CI4" s="599"/>
-      <c r="CJ4" s="599"/>
-      <c r="CK4" s="600"/>
+      <c r="CH4" s="606"/>
+      <c r="CI4" s="606"/>
+      <c r="CJ4" s="606"/>
+      <c r="CK4" s="607"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" s="359"/>
@@ -66540,6 +66516,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -66552,11 +66533,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Space Cooling Projections from PoTenCIA
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRes_RSD_NewTechs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1307D6-DD79-43FD-9081-58A0901E9B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC786213-D949-4A71-A94C-AA6D1CA99EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34F9D92C-266F-476D-89E0-63153305AC39}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -45,15 +45,31 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={EFB69185-C1DE-40F7-8616-8CF0AAA0F16E}</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{EFB69185-C1DE-40F7-8616-8CF0AAA0F16E}">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{55B70DE9-B746-4DBB-9879-ABAEC3E40522}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Assumption - Half of Pumps&amp;Fan Energy is Cooling Energy</t>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+As per PoTENCIA projections X dwelling factor</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -12323,7 +12339,7 @@
     <numFmt numFmtId="172" formatCode="0.000"/>
     <numFmt numFmtId="173" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="74" x14ac:knownFonts="1">
+  <fonts count="76" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -12800,6 +12816,19 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="39">
@@ -15269,6 +15298,15 @@
     <xf numFmtId="0" fontId="54" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -15276,15 +15314,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15296,17 +15325,26 @@
     <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -15317,19 +15355,10 @@
     <xf numFmtId="0" fontId="70" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15347,12 +15376,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -15367,6 +15390,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -16597,6 +16626,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16916,14 +16949,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I7" dT="2021-01-21T15:17:09.58" personId="{00000000-0000-0000-0000-000000000000}" id="{EFB69185-C1DE-40F7-8616-8CF0AAA0F16E}">
-    <text>Assumption - Half of Pumps&amp;Fan Energy is Cooling Energy</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet10">
@@ -17391,23 +17416,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="611" t="s">
+      <c r="A1" s="609" t="s">
         <v>1062</v>
       </c>
-      <c r="B1" s="613" t="s">
+      <c r="B1" s="611" t="s">
         <v>1063</v>
       </c>
-      <c r="C1" s="614"/>
-      <c r="D1" s="614"/>
-      <c r="E1" s="614"/>
-      <c r="F1" s="615"/>
-      <c r="G1" s="613" t="s">
+      <c r="C1" s="612"/>
+      <c r="D1" s="612"/>
+      <c r="E1" s="612"/>
+      <c r="F1" s="613"/>
+      <c r="G1" s="611" t="s">
         <v>1064</v>
       </c>
-      <c r="H1" s="614"/>
-      <c r="I1" s="614"/>
-      <c r="J1" s="614"/>
-      <c r="K1" s="615"/>
+      <c r="H1" s="612"/>
+      <c r="I1" s="612"/>
+      <c r="J1" s="612"/>
+      <c r="K1" s="613"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -17417,7 +17442,7 @@
       <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="612"/>
+      <c r="A2" s="610"/>
       <c r="B2" s="527" t="s">
         <v>686</v>
       </c>
@@ -18910,11 +18935,11 @@
       <c r="Y48" t="s">
         <v>1113</v>
       </c>
-      <c r="Z48" s="609" t="s">
+      <c r="Z48" s="614" t="s">
         <v>1051</v>
       </c>
-      <c r="AA48" s="610"/>
-      <c r="AB48" s="610"/>
+      <c r="AA48" s="615"/>
+      <c r="AB48" s="615"/>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -19131,11 +19156,11 @@
       <c r="Y53" t="s">
         <v>1115</v>
       </c>
-      <c r="Z53" s="609" t="s">
+      <c r="Z53" s="614" t="s">
         <v>1050</v>
       </c>
-      <c r="AA53" s="610"/>
-      <c r="AB53" s="610"/>
+      <c r="AA53" s="615"/>
+      <c r="AB53" s="615"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -19342,11 +19367,11 @@
       <c r="Y59" t="s">
         <v>1116</v>
       </c>
-      <c r="Z59" s="609" t="s">
+      <c r="Z59" s="614" t="s">
         <v>1117</v>
       </c>
-      <c r="AA59" s="610"/>
-      <c r="AB59" s="610"/>
+      <c r="AA59" s="615"/>
+      <c r="AB59" s="615"/>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="547" t="str">
@@ -20244,17 +20269,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="Z59:AB59"/>
+    <mergeCell ref="Z53:AB53"/>
+    <mergeCell ref="Z48:AB48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="Z59:AB59"/>
-    <mergeCell ref="Z53:AB53"/>
-    <mergeCell ref="Z48:AB48"/>
   </mergeCells>
   <phoneticPr fontId="71" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21007,7 +21032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4660B878-9B9C-4131-8EFF-29EF25ED69C5}">
   <dimension ref="A2:AL103"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -21207,8 +21232,8 @@
       <c r="G7" s="71"/>
       <c r="H7" s="109"/>
       <c r="I7" s="314">
-        <f>(AK23*N11)/2</f>
-        <v>2.1494423184792772E-4</v>
+        <f>0.000214944231847928*0.9</f>
+        <v>1.934498086631352E-4</v>
       </c>
       <c r="J7" s="103"/>
       <c r="S7" s="300" t="s">
@@ -21303,8 +21328,8 @@
       <c r="G10" s="166"/>
       <c r="H10" s="132"/>
       <c r="I10" s="316">
-        <f>(AK23*N11)/2</f>
-        <v>2.1494423184792772E-4</v>
+        <f>(AK23*N11)</f>
+        <v>4.2988846369585544E-4</v>
       </c>
       <c r="J10" s="141"/>
       <c r="M10" s="291" t="s">
@@ -21420,8 +21445,7 @@
       <c r="G13" s="71"/>
       <c r="H13" s="109"/>
       <c r="I13" s="314">
-        <f>(AK37*N11)/2</f>
-        <v>3.7440784810945435E-4</v>
+        <v>2.1494423184792772E-4</v>
       </c>
       <c r="J13" s="103"/>
       <c r="S13" s="303" t="s">
@@ -21507,8 +21531,8 @@
       <c r="G16" s="166"/>
       <c r="H16" s="132"/>
       <c r="I16" s="316">
-        <f>(AK37*N11)/2</f>
-        <v>3.7440784810945435E-4</v>
+        <f>(AK37*N11)</f>
+        <v>7.488156962189087E-4</v>
       </c>
       <c r="J16" s="141"/>
     </row>
@@ -21567,8 +21591,8 @@
       <c r="G19" s="71"/>
       <c r="H19" s="109"/>
       <c r="I19" s="314">
-        <f>(AK52*N11)/2</f>
-        <v>3.9601185380309516E-4</v>
+        <f>0.000214944231847928*1.1</f>
+        <v>2.364386550327208E-4</v>
       </c>
       <c r="J19" s="103"/>
     </row>
@@ -21693,8 +21717,8 @@
       <c r="G22" s="166"/>
       <c r="H22" s="132"/>
       <c r="I22" s="316">
-        <f>(AK52*N11)/2</f>
-        <v>3.9601185380309516E-4</v>
+        <f>(AK52*N11)</f>
+        <v>7.9202370760619032E-4</v>
       </c>
       <c r="J22" s="141"/>
       <c r="V22" s="5" t="s">
@@ -28776,7 +28800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F8057-C735-4662-BAA6-EEDCF7B57273}">
   <dimension ref="A2:AR166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
@@ -28963,12 +28987,12 @@
         <v>321</v>
       </c>
       <c r="U4" s="591"/>
-      <c r="V4" s="592" t="s">
+      <c r="V4" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="W4" s="593"/>
-      <c r="X4" s="593"/>
-      <c r="Y4" s="594"/>
+      <c r="W4" s="584"/>
+      <c r="X4" s="584"/>
+      <c r="Y4" s="585"/>
       <c r="Z4" s="106"/>
       <c r="AA4" s="106"/>
       <c r="AB4" s="114" t="s">
@@ -29067,34 +29091,34 @@
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
       <c r="G6" s="85"/>
-      <c r="H6" s="583" t="s">
+      <c r="H6" s="586" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="584"/>
-      <c r="J6" s="584"/>
-      <c r="K6" s="585"/>
-      <c r="L6" s="584" t="s">
+      <c r="I6" s="587"/>
+      <c r="J6" s="587"/>
+      <c r="K6" s="588"/>
+      <c r="L6" s="587" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="584"/>
-      <c r="N6" s="584"/>
-      <c r="O6" s="585"/>
-      <c r="P6" s="583" t="s">
+      <c r="M6" s="587"/>
+      <c r="N6" s="587"/>
+      <c r="O6" s="588"/>
+      <c r="P6" s="586" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="584"/>
-      <c r="R6" s="584"/>
-      <c r="S6" s="585"/>
-      <c r="T6" s="583" t="s">
+      <c r="Q6" s="587"/>
+      <c r="R6" s="587"/>
+      <c r="S6" s="588"/>
+      <c r="T6" s="586" t="s">
         <v>302</v>
       </c>
-      <c r="U6" s="585"/>
-      <c r="V6" s="583" t="s">
+      <c r="U6" s="588"/>
+      <c r="V6" s="586" t="s">
         <v>967</v>
       </c>
-      <c r="W6" s="584"/>
-      <c r="X6" s="584"/>
-      <c r="Y6" s="585"/>
+      <c r="W6" s="587"/>
+      <c r="X6" s="587"/>
+      <c r="Y6" s="588"/>
       <c r="Z6" s="107" t="s">
         <v>979</v>
       </c>
@@ -32113,12 +32137,12 @@
         <v>321</v>
       </c>
       <c r="U42" s="591"/>
-      <c r="V42" s="592" t="s">
+      <c r="V42" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="W42" s="593"/>
-      <c r="X42" s="593"/>
-      <c r="Y42" s="594"/>
+      <c r="W42" s="584"/>
+      <c r="X42" s="584"/>
+      <c r="Y42" s="585"/>
       <c r="Z42" s="106"/>
       <c r="AA42" s="106"/>
       <c r="AB42" s="114" t="s">
@@ -32217,34 +32241,34 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="85"/>
-      <c r="H44" s="583" t="s">
+      <c r="H44" s="586" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="584"/>
-      <c r="J44" s="584"/>
-      <c r="K44" s="585"/>
-      <c r="L44" s="584" t="s">
+      <c r="I44" s="587"/>
+      <c r="J44" s="587"/>
+      <c r="K44" s="588"/>
+      <c r="L44" s="587" t="s">
         <v>45</v>
       </c>
-      <c r="M44" s="584"/>
-      <c r="N44" s="584"/>
-      <c r="O44" s="585"/>
-      <c r="P44" s="583" t="s">
+      <c r="M44" s="587"/>
+      <c r="N44" s="587"/>
+      <c r="O44" s="588"/>
+      <c r="P44" s="586" t="s">
         <v>45</v>
       </c>
-      <c r="Q44" s="584"/>
-      <c r="R44" s="584"/>
-      <c r="S44" s="585"/>
-      <c r="T44" s="586" t="s">
+      <c r="Q44" s="587"/>
+      <c r="R44" s="587"/>
+      <c r="S44" s="588"/>
+      <c r="T44" s="592" t="s">
         <v>302</v>
       </c>
-      <c r="U44" s="587"/>
-      <c r="V44" s="586" t="s">
+      <c r="U44" s="593"/>
+      <c r="V44" s="592" t="s">
         <v>967</v>
       </c>
-      <c r="W44" s="588"/>
-      <c r="X44" s="588"/>
-      <c r="Y44" s="587"/>
+      <c r="W44" s="594"/>
+      <c r="X44" s="594"/>
+      <c r="Y44" s="593"/>
       <c r="Z44" s="450" t="s">
         <v>979</v>
       </c>
@@ -36023,12 +36047,12 @@
         <v>321</v>
       </c>
       <c r="U90" s="591"/>
-      <c r="V90" s="592" t="s">
+      <c r="V90" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="W90" s="593"/>
-      <c r="X90" s="593"/>
-      <c r="Y90" s="594"/>
+      <c r="W90" s="584"/>
+      <c r="X90" s="584"/>
+      <c r="Y90" s="585"/>
       <c r="Z90" s="106"/>
       <c r="AA90" s="106"/>
       <c r="AB90" s="114" t="s">
@@ -36127,34 +36151,34 @@
       <c r="E92" s="84"/>
       <c r="F92" s="84"/>
       <c r="G92" s="85"/>
-      <c r="H92" s="583" t="s">
+      <c r="H92" s="586" t="s">
         <v>45</v>
       </c>
-      <c r="I92" s="584"/>
-      <c r="J92" s="584"/>
-      <c r="K92" s="585"/>
-      <c r="L92" s="584" t="s">
+      <c r="I92" s="587"/>
+      <c r="J92" s="587"/>
+      <c r="K92" s="588"/>
+      <c r="L92" s="587" t="s">
         <v>45</v>
       </c>
-      <c r="M92" s="584"/>
-      <c r="N92" s="584"/>
-      <c r="O92" s="585"/>
-      <c r="P92" s="583" t="s">
+      <c r="M92" s="587"/>
+      <c r="N92" s="587"/>
+      <c r="O92" s="588"/>
+      <c r="P92" s="586" t="s">
         <v>45</v>
       </c>
-      <c r="Q92" s="584"/>
-      <c r="R92" s="584"/>
-      <c r="S92" s="585"/>
-      <c r="T92" s="586" t="s">
+      <c r="Q92" s="587"/>
+      <c r="R92" s="587"/>
+      <c r="S92" s="588"/>
+      <c r="T92" s="592" t="s">
         <v>302</v>
       </c>
-      <c r="U92" s="587"/>
-      <c r="V92" s="586" t="s">
+      <c r="U92" s="593"/>
+      <c r="V92" s="592" t="s">
         <v>967</v>
       </c>
-      <c r="W92" s="588"/>
-      <c r="X92" s="588"/>
-      <c r="Y92" s="587"/>
+      <c r="W92" s="594"/>
+      <c r="X92" s="594"/>
+      <c r="Y92" s="593"/>
       <c r="Z92" s="450" t="s">
         <v>979</v>
       </c>
@@ -40073,6 +40097,26 @@
     <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="L92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="V92:Y92"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="L90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="T90:U90"/>
+    <mergeCell ref="V90:Y90"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:Y44"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:O42"/>
+    <mergeCell ref="P42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:Y42"/>
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V6:Y6"/>
     <mergeCell ref="H4:K4"/>
@@ -40083,26 +40127,6 @@
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:O42"/>
-    <mergeCell ref="P42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="L90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="T90:U90"/>
-    <mergeCell ref="V90:Y90"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="L92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="T92:U92"/>
-    <mergeCell ref="V92:Y92"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -40247,12 +40271,12 @@
       <c r="I5" s="173"/>
       <c r="J5" s="173"/>
       <c r="K5" s="173"/>
-      <c r="L5" s="592" t="s">
+      <c r="L5" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="593"/>
-      <c r="N5" s="593"/>
-      <c r="O5" s="594"/>
+      <c r="M5" s="584"/>
+      <c r="N5" s="584"/>
+      <c r="O5" s="585"/>
       <c r="P5" s="106"/>
       <c r="Q5" s="106" t="s">
         <v>323</v>
@@ -40283,12 +40307,12 @@
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
       <c r="K6" s="83"/>
-      <c r="L6" s="586" t="s">
+      <c r="L6" s="592" t="s">
         <v>967</v>
       </c>
-      <c r="M6" s="588"/>
-      <c r="N6" s="588"/>
-      <c r="O6" s="587"/>
+      <c r="M6" s="594"/>
+      <c r="N6" s="594"/>
+      <c r="O6" s="593"/>
       <c r="P6" s="450" t="s">
         <v>979</v>
       </c>
@@ -41206,23 +41230,23 @@
       <c r="K33" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L33" s="592" t="s">
+      <c r="L33" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="M33" s="593"/>
-      <c r="N33" s="593"/>
-      <c r="O33" s="594"/>
+      <c r="M33" s="584"/>
+      <c r="N33" s="584"/>
+      <c r="O33" s="585"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H34" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L34" s="586" t="s">
+      <c r="L34" s="592" t="s">
         <v>327</v>
       </c>
-      <c r="M34" s="588"/>
-      <c r="N34" s="588"/>
-      <c r="O34" s="587"/>
+      <c r="M34" s="594"/>
+      <c r="N34" s="594"/>
+      <c r="O34" s="593"/>
     </row>
     <row r="35" spans="8:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5" t="s">
@@ -41569,11 +41593,11 @@
       </c>
       <c r="I4" s="590"/>
       <c r="J4" s="591"/>
-      <c r="K4" s="592" t="s">
+      <c r="K4" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="L4" s="593"/>
-      <c r="M4" s="594"/>
+      <c r="L4" s="584"/>
+      <c r="M4" s="585"/>
       <c r="N4" s="106"/>
       <c r="O4" s="106" t="s">
         <v>323</v>
@@ -41599,16 +41623,16 @@
       <c r="G5" s="458" t="s">
         <v>302</v>
       </c>
-      <c r="H5" s="599" t="s">
+      <c r="H5" s="596" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="600"/>
-      <c r="J5" s="601"/>
-      <c r="K5" s="599" t="s">
+      <c r="I5" s="597"/>
+      <c r="J5" s="598"/>
+      <c r="K5" s="596" t="s">
         <v>756</v>
       </c>
-      <c r="L5" s="600"/>
-      <c r="M5" s="601"/>
+      <c r="L5" s="597"/>
+      <c r="M5" s="598"/>
       <c r="N5" s="459" t="s">
         <v>328</v>
       </c>
@@ -41625,23 +41649,23 @@
         <v>626</v>
       </c>
       <c r="AA5" s="281"/>
-      <c r="AB5" s="596" t="s">
+      <c r="AB5" s="599" t="s">
         <v>1011</v>
       </c>
-      <c r="AC5" s="596"/>
+      <c r="AC5" s="599"/>
       <c r="AD5" s="461"/>
-      <c r="AE5" s="597" t="s">
+      <c r="AE5" s="600" t="s">
         <v>110</v>
       </c>
-      <c r="AF5" s="597"/>
-      <c r="AG5" s="597" t="s">
+      <c r="AF5" s="600"/>
+      <c r="AG5" s="600" t="s">
         <v>1012</v>
       </c>
-      <c r="AH5" s="597"/>
-      <c r="AI5" s="598" t="s">
+      <c r="AH5" s="600"/>
+      <c r="AI5" s="601" t="s">
         <v>1013</v>
       </c>
-      <c r="AJ5" s="598"/>
+      <c r="AJ5" s="601"/>
     </row>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C6" s="505" t="str">
@@ -42379,12 +42403,12 @@
       <c r="K27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="592" t="s">
+      <c r="L27" s="583" t="s">
         <v>322</v>
       </c>
-      <c r="M27" s="593"/>
-      <c r="N27" s="593"/>
-      <c r="O27" s="594"/>
+      <c r="M27" s="584"/>
+      <c r="N27" s="584"/>
+      <c r="O27" s="585"/>
       <c r="T27" s="283"/>
       <c r="U27" s="283"/>
     </row>
@@ -42392,12 +42416,12 @@
       <c r="J28" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="L28" s="583" t="s">
+      <c r="L28" s="586" t="s">
         <v>327</v>
       </c>
-      <c r="M28" s="584"/>
-      <c r="N28" s="584"/>
-      <c r="O28" s="585"/>
+      <c r="M28" s="587"/>
+      <c r="N28" s="587"/>
+      <c r="O28" s="588"/>
       <c r="T28" s="283"/>
       <c r="U28" s="283"/>
     </row>
@@ -43787,16 +43811,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="L27:O27"/>
     <mergeCell ref="L28:O28"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="L27:O27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="S7" r:id="rId1" xr:uid="{B1EDD63D-40A5-4174-9D28-8666BD314B83}"/>
@@ -52826,103 +52850,103 @@
       <c r="C4" s="356" t="s">
         <v>765</v>
       </c>
-      <c r="D4" s="603" t="s">
+      <c r="D4" s="602" t="s">
         <v>766</v>
       </c>
-      <c r="E4" s="602"/>
-      <c r="F4" s="602"/>
-      <c r="G4" s="602"/>
+      <c r="E4" s="603"/>
+      <c r="F4" s="603"/>
+      <c r="G4" s="603"/>
       <c r="H4" s="604"/>
-      <c r="I4" s="602" t="s">
+      <c r="I4" s="603" t="s">
         <v>767</v>
       </c>
-      <c r="J4" s="602"/>
-      <c r="K4" s="602"/>
-      <c r="L4" s="602"/>
+      <c r="J4" s="603"/>
+      <c r="K4" s="603"/>
+      <c r="L4" s="603"/>
       <c r="M4" s="604"/>
-      <c r="N4" s="602" t="s">
+      <c r="N4" s="603" t="s">
         <v>768</v>
       </c>
-      <c r="O4" s="602"/>
-      <c r="P4" s="602"/>
-      <c r="Q4" s="602"/>
+      <c r="O4" s="603"/>
+      <c r="P4" s="603"/>
+      <c r="Q4" s="603"/>
       <c r="R4" s="604"/>
-      <c r="S4" s="602" t="s">
+      <c r="S4" s="603" t="s">
         <v>769</v>
       </c>
-      <c r="T4" s="602"/>
-      <c r="U4" s="602"/>
-      <c r="V4" s="602"/>
+      <c r="T4" s="603"/>
+      <c r="U4" s="603"/>
+      <c r="V4" s="603"/>
       <c r="W4" s="604"/>
-      <c r="X4" s="602" t="s">
+      <c r="X4" s="603" t="s">
         <v>770</v>
       </c>
-      <c r="Y4" s="602"/>
-      <c r="Z4" s="602"/>
-      <c r="AA4" s="602"/>
+      <c r="Y4" s="603"/>
+      <c r="Z4" s="603"/>
+      <c r="AA4" s="603"/>
       <c r="AB4" s="604"/>
-      <c r="AC4" s="602" t="s">
+      <c r="AC4" s="603" t="s">
         <v>771</v>
       </c>
-      <c r="AD4" s="602"/>
-      <c r="AE4" s="602"/>
-      <c r="AF4" s="602"/>
+      <c r="AD4" s="603"/>
+      <c r="AE4" s="603"/>
+      <c r="AF4" s="603"/>
       <c r="AG4" s="604"/>
-      <c r="AH4" s="602" t="s">
+      <c r="AH4" s="603" t="s">
         <v>772</v>
       </c>
-      <c r="AI4" s="602"/>
-      <c r="AJ4" s="602"/>
-      <c r="AK4" s="602"/>
+      <c r="AI4" s="603"/>
+      <c r="AJ4" s="603"/>
+      <c r="AK4" s="603"/>
       <c r="AL4" s="604"/>
-      <c r="AM4" s="602" t="s">
+      <c r="AM4" s="603" t="s">
         <v>773</v>
       </c>
-      <c r="AN4" s="602"/>
-      <c r="AO4" s="602"/>
-      <c r="AP4" s="602"/>
+      <c r="AN4" s="603"/>
+      <c r="AO4" s="603"/>
+      <c r="AP4" s="603"/>
       <c r="AQ4" s="604"/>
-      <c r="AR4" s="602" t="s">
+      <c r="AR4" s="603" t="s">
         <v>774</v>
       </c>
-      <c r="AS4" s="602"/>
-      <c r="AT4" s="602"/>
-      <c r="AU4" s="602"/>
+      <c r="AS4" s="603"/>
+      <c r="AT4" s="603"/>
+      <c r="AU4" s="603"/>
       <c r="AV4" s="604"/>
-      <c r="AW4" s="602" t="s">
+      <c r="AW4" s="603" t="s">
         <v>775</v>
       </c>
-      <c r="AX4" s="602"/>
-      <c r="AY4" s="602"/>
-      <c r="AZ4" s="602"/>
-      <c r="BA4" s="602"/>
-      <c r="BB4" s="603" t="s">
+      <c r="AX4" s="603"/>
+      <c r="AY4" s="603"/>
+      <c r="AZ4" s="603"/>
+      <c r="BA4" s="603"/>
+      <c r="BB4" s="602" t="s">
         <v>776</v>
       </c>
-      <c r="BC4" s="602"/>
-      <c r="BD4" s="602"/>
-      <c r="BE4" s="602"/>
+      <c r="BC4" s="603"/>
+      <c r="BD4" s="603"/>
+      <c r="BE4" s="603"/>
       <c r="BF4" s="604"/>
-      <c r="BG4" s="602" t="s">
+      <c r="BG4" s="603" t="s">
         <v>777</v>
       </c>
-      <c r="BH4" s="602"/>
-      <c r="BI4" s="602"/>
-      <c r="BJ4" s="602"/>
-      <c r="BK4" s="602"/>
-      <c r="BL4" s="603" t="s">
+      <c r="BH4" s="603"/>
+      <c r="BI4" s="603"/>
+      <c r="BJ4" s="603"/>
+      <c r="BK4" s="603"/>
+      <c r="BL4" s="602" t="s">
         <v>778</v>
       </c>
-      <c r="BM4" s="602"/>
-      <c r="BN4" s="602"/>
-      <c r="BO4" s="602"/>
-      <c r="BP4" s="602"/>
-      <c r="BQ4" s="603" t="s">
+      <c r="BM4" s="603"/>
+      <c r="BN4" s="603"/>
+      <c r="BO4" s="603"/>
+      <c r="BP4" s="603"/>
+      <c r="BQ4" s="602" t="s">
         <v>779</v>
       </c>
-      <c r="BR4" s="602"/>
-      <c r="BS4" s="602"/>
-      <c r="BT4" s="602"/>
+      <c r="BR4" s="603"/>
+      <c r="BS4" s="603"/>
+      <c r="BT4" s="603"/>
       <c r="BU4" s="604"/>
       <c r="BV4" s="357" t="s">
         <v>780</v>
@@ -66516,11 +66540,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -66533,6 +66552,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>